<commit_message>
Updated registers for 2-channel differential with correct bias settings.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoodms\Documents\_APPDEV_new\nRF_Development\nRF5_SDK_11.0.0_2\examples\_my_projects\EEG_ADS1299_Firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoodms\Documents\_APPDEV_new\nRF_Development\nRF5_SDK_11.0.0_2\examples\_my_projects\nRF51_EOG_ADS1299_Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>ADDRESS</t>
   </si>
@@ -227,9 +227,6 @@
     <t>EXPERIMENT WITH LOFF LATER; WHEN EVERYTHING ELSE WORKS: CREATE NEW CHARACTERISTIC FOR IT</t>
   </si>
   <si>
-    <t>Channel power down, disable gain, SRB2 open (not connected),</t>
-  </si>
-  <si>
     <t>Normal electrode, enabled, G=24, SRB2 open</t>
   </si>
   <si>
@@ -261,13 +258,16 @@
   </si>
   <si>
     <t>CHECKID</t>
+  </si>
+  <si>
+    <t>Disabled Channels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +313,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -386,7 +394,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -418,6 +426,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -706,7 +719,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +727,7 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34.140625" customWidth="1"/>
-    <col min="18" max="18" width="37.85546875" customWidth="1"/>
+    <col min="18" max="18" width="4" customWidth="1"/>
     <col min="19" max="19" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -939,14 +952,14 @@
         <v>66</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C6" t="str">
@@ -981,17 +994,17 @@
         <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="str">
@@ -1025,90 +1038,99 @@
       <c r="L7" s="4">
         <v>49</v>
       </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>0x60</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
+      <c r="C8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11">
+        <v>1</v>
       </c>
       <c r="L8" s="4">
         <v>49</v>
       </c>
+      <c r="M8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>0x60</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
+      <c r="C9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1</v>
       </c>
       <c r="L9" s="4">
         <v>49</v>
+      </c>
+      <c r="M9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="10" t="str">
@@ -1143,14 +1165,14 @@
         <v>49</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="10" t="str">
@@ -1183,13 +1205,16 @@
       </c>
       <c r="L11" s="4">
         <v>49</v>
+      </c>
+      <c r="M11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="10" t="str">
@@ -1222,13 +1247,16 @@
       </c>
       <c r="L12" s="4">
         <v>49</v>
+      </c>
+      <c r="M12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="10" t="str">
@@ -1261,18 +1289,21 @@
       </c>
       <c r="L13" s="4">
         <v>49</v>
+      </c>
+      <c r="M13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>0x0F</v>
+        <v>0x03</v>
       </c>
       <c r="D14" s="11">
         <v>0</v>
@@ -1287,10 +1318,10 @@
         <v>0</v>
       </c>
       <c r="H14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -1302,19 +1333,19 @@
         <v>50</v>
       </c>
       <c r="M14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>0x00</v>
+        <v>0x03</v>
       </c>
       <c r="D15" s="11">
         <v>0</v>
@@ -1335,23 +1366,23 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
@@ -1367,33 +1398,33 @@
       <c r="G16" s="11">
         <v>0</v>
       </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
         <v>52</v>
       </c>
-      <c r="M16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="M16" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
@@ -1409,30 +1440,30 @@
       <c r="G17" s="11">
         <v>0</v>
       </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="10" t="str">
         <f t="shared" si="0"/>
         <v>0x00</v>
       </c>
@@ -1448,19 +1479,19 @@
       <c r="G18" s="11">
         <v>0</v>
       </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
         <v>54</v>
       </c>
     </row>
@@ -1503,10 +1534,10 @@
         <v>55</v>
       </c>
       <c r="M19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1548,49 +1579,49 @@
         <v>56</v>
       </c>
       <c r="M20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0F</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <v>0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+      <c r="H21" s="15">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15">
+        <v>1</v>
+      </c>
+      <c r="J21" s="15">
+        <v>1</v>
+      </c>
+      <c r="K21" s="15">
+        <v>1</v>
+      </c>
+      <c r="L21" s="11">
+        <v>57</v>
+      </c>
+      <c r="M21" s="10" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>0x0F</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7">
-        <v>0</v>
-      </c>
-      <c r="H21" s="7">
-        <v>1</v>
-      </c>
-      <c r="I21" s="7">
-        <v>1</v>
-      </c>
-      <c r="J21" s="7">
-        <v>1</v>
-      </c>
-      <c r="K21" s="7">
-        <v>1</v>
-      </c>
-      <c r="L21" s="4">
-        <v>57</v>
-      </c>
-      <c r="M21" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1602,7 +1633,7 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>0x20</v>
+        <v>0x00</v>
       </c>
       <c r="D22" s="6">
         <v>0</v>
@@ -1611,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="6">
         <v>0</v>
@@ -1632,7 +1663,7 @@
         <v>58</v>
       </c>
       <c r="M22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1713,12 +1744,12 @@
         <v>59</v>
       </c>
       <c r="M24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" ref="C26" si="1">"0x"&amp;TEXT(DEC2HEX(K26+2*J26+4*I26+8*H26+16*G26+32*F26+64*E26+128*D26,2),"00")</f>

</xml_diff>